<commit_message>
Checking in after fix
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDriver/TestSBO_Replay_M1/Test.xlsx
+++ b/src/test/resources/TestDriver/TestSBO_Replay_M1/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arahmed\OneDrive - SS&amp;C Technologies, Inc\Desktop\Pers\fyntrac-data-main\fyntrac-data-main\src\test\resources\TestDriver\TestSBO_Replay_M1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4C5D8F-E2F7-4BBE-AC6A-1CE79745B1CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638055A3-D711-4CA1-B436-17D74F24BA4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
@@ -132,9 +132,6 @@
     <t>ETL</t>
   </si>
   <si>
-    <t>LOAN1</t>
-  </si>
-  <si>
     <t>TestSBO_Replay_M1/ReferenceData/RefData_SBO_EVENTS.xlsx</t>
   </si>
   <si>
@@ -169,6 +166,9 @@
   </si>
   <si>
     <t>{"instrumentId": "IDHJ-EGNY"}</t>
+  </si>
+  <si>
+    <t>IDHJ-EGNY</t>
   </si>
 </sst>
 </file>
@@ -493,7 +493,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -504,7 +504,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -515,7 +515,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -537,7 +537,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -570,7 +570,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -603,7 +603,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -625,7 +625,7 @@
         <v>4</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -669,7 +669,7 @@
         <v>4</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -697,9 +697,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -714,7 +712,7 @@
         <v>13</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G1" s="5"/>
     </row>
@@ -738,7 +736,7 @@
         <v>19</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>20</v>
@@ -767,7 +765,7 @@
         <v>20220131</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="G3" s="8">
         <v>100</v>
@@ -799,7 +797,7 @@
         <v>20220131</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="G4" s="8">
         <v>100000</v>
@@ -831,7 +829,7 @@
         <v>20220201</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="G5" s="8">
         <v>27.777799999999999</v>
@@ -863,7 +861,7 @@
         <v>20220202</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="G6" s="8">
         <v>27.777799999999999</v>
@@ -895,7 +893,7 @@
         <v>20220203</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="G7" s="8">
         <v>-80</v>
@@ -927,7 +925,7 @@
         <v>20220203</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="G8" s="8">
         <v>80</v>
@@ -959,7 +957,7 @@
         <v>20220203</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="G9" s="8">
         <v>27.777799999999999</v>
@@ -991,7 +989,7 @@
         <v>20220204</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="G10" s="8">
         <v>27.777799999999999</v>
@@ -1023,7 +1021,7 @@
         <v>20220205</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="G11" s="8">
         <v>-131.1112</v>
@@ -1055,7 +1053,7 @@
         <v>20220205</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="G12" s="8">
         <v>-143.8888</v>
@@ -1087,7 +1085,7 @@
         <v>20220205</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="G13" s="8">
         <v>275</v>
@@ -1119,7 +1117,7 @@
         <v>20220205</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="G14" s="8">
         <v>27.7378</v>
@@ -1151,7 +1149,7 @@
         <v>20220206</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="G15" s="8">
         <v>-27.7378</v>
@@ -1183,7 +1181,7 @@
         <v>20220206</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="G16" s="8">
         <v>-322.26220000000001</v>
@@ -1215,7 +1213,7 @@
         <v>20220206</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="G17" s="8">
         <v>350</v>
@@ -1247,7 +1245,7 @@
         <v>20220206</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="G18" s="8">
         <v>27.648299999999999</v>
@@ -1279,7 +1277,7 @@
         <v>20220207</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="G19" s="8">
         <v>27.648299999999999</v>
@@ -1311,7 +1309,7 @@
         <v>20220208</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="G20" s="8">
         <v>27.648299999999999</v>
@@ -1334,7 +1332,7 @@
         <v>1</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>24</v>
@@ -1343,7 +1341,7 @@
         <v>20220209</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="G21" s="8">
         <v>3.3300000000000003E-2</v>
@@ -1366,7 +1364,7 @@
         <v>1</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>24</v>
@@ -1375,7 +1373,7 @@
         <v>20220209</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="G22" s="8">
         <v>30.008299999999998</v>
@@ -1407,7 +1405,7 @@
         <v>20220203</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="G23" s="8">
         <v>-30</v>
@@ -1439,7 +1437,7 @@
         <v>20220209</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="G24" s="8">
         <v>27.648299999999999</v>

</xml_diff>